<commit_message>
Performance average for 256 simulations workflow
</commit_message>
<xml_diff>
--- a/viveks_workflow/analysis/integration_analysis.xlsx
+++ b/viveks_workflow/analysis/integration_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TTC" sheetId="1" r:id="rId1"/>
@@ -4833,8 +4833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4892,22 +4892,22 @@
       </c>
       <c r="H2" s="6">
         <f>AVERAGE(H4:H11)</f>
-        <v>23.884344544741584</v>
+        <v>17.316149794937647</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="M2" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N2" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O2" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P2" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q2" s="9"/>
     </row>
@@ -4925,7 +4925,7 @@
       <c r="F3" s="5"/>
       <c r="H3" s="7">
         <f>_xlfn.STDEV.S(H4:H11)</f>
-        <v>3.8713434740789232</v>
+        <v>2.8067240187072193</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
@@ -4943,23 +4943,23 @@
         <v>5525</v>
       </c>
       <c r="H4" s="8">
-        <f>(O4/B4)*100</f>
-        <v>21.719457013574662</v>
+        <f>(M4/B4)*100</f>
+        <v>15.746606334841628</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="M4" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N4" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O4" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P4" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q4" s="9"/>
     </row>
@@ -4971,23 +4971,23 @@
         <v>4052</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" ref="H5:K11" si="0">(O5/B5)*100</f>
-        <v>29.615004935834154</v>
+        <f t="shared" ref="H5:H11" si="0">(M5/B5)*100</f>
+        <v>21.470878578479763</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="M5" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N5" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O5" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P5" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q5" s="9"/>
     </row>
@@ -5000,22 +5000,22 @@
       </c>
       <c r="H6" s="8">
         <f t="shared" si="0"/>
-        <v>22.835394862036157</v>
+        <v>16.555661274976213</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="M6" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N6" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O6" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P6" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q6" s="9"/>
     </row>
@@ -5028,22 +5028,22 @@
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
-        <v>21.367521367521366</v>
+        <v>15.491452991452991</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="M7" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N7" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O7" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P7" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
@@ -5056,16 +5056,16 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="M8" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N8" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O8" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P8" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q8" s="9"/>
     </row>
@@ -5077,16 +5077,16 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="M9" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N9" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O9" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P9" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q9" s="9"/>
     </row>
@@ -5098,16 +5098,16 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="M10" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N10" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O10" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P10" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q10" s="9"/>
     </row>
@@ -5115,18 +5115,19 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="M11" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="N11" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="O11" s="9">
-        <v>1200</v>
+        <v>870</v>
       </c>
       <c r="P11" s="9">
-        <v>2400</v>
+        <v>870</v>
       </c>
       <c r="Q11" s="9"/>
     </row>
@@ -5140,7 +5141,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5246,7 +5247,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5351,7 +5352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:A35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Analysis 1024 simulations integrated experiments
</commit_message>
<xml_diff>
--- a/viveks_workflow/analysis/integration_analysis.xlsx
+++ b/viveks_workflow/analysis/integration_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TTC" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,11 @@
   </externalReferences>
   <definedNames>
     <definedName name="Te_Executing_task_aimes_emgr" localSheetId="2">Te!$B$4:$B$7</definedName>
+    <definedName name="Te_Executing_task_aimes_emgr_1" localSheetId="2">Te!$D$4:$D$6</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr" localSheetId="0">TTC!$B$4:$B$7</definedName>
+    <definedName name="TTC_Time_to_completion_aimes_emgr_1" localSheetId="0">TTC!$D$4:$D$6</definedName>
     <definedName name="Tw_Submitting_task_aimes_emgr" localSheetId="1">Tw!$B$4:$B$7</definedName>
+    <definedName name="Tw_Submitting_task_aimes_emgr_1" localSheetId="1">Tw!$D$4:$D$6</definedName>
   </definedNames>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -46,15 +49,36 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="TTC-Time_to_completion-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="2" name="Te-Executing_task-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/Te-Executing_task-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="TTC-Time_to_completion-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="Tw-Submitting_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="4" name="TTC-Time_to_completion-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/TTC-Time_to_completion-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="Tw-Submitting_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/Tw-Submitting_task-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="Tw-Submitting_task-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/Tw-Submitting_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
@@ -191,13 +215,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -281,6 +304,9 @@
                   <c:pt idx="0">
                     <c:v>723.1030355350474</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>81.79445783996207</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -292,6 +318,9 @@
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
                     <c:v>723.1030355350474</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>81.79445783996207</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -339,6 +368,9 @@
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5112.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10089.33333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -804,6 +836,9 @@
                   <c:pt idx="0">
                     <c:v>890.7451936440634</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>393.1602726624347</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -815,6 +850,9 @@
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
                     <c:v>890.7451936440634</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>393.1602726624347</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -862,6 +900,9 @@
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3692.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7165.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1250,6 +1291,9 @@
                   <c:pt idx="0">
                     <c:v>775.6100287300743</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>89.62886439832501</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -1261,6 +1305,9 @@
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
                     <c:v>775.6100287300743</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>89.62886439832501</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1308,6 +1355,9 @@
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4535.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9868.666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1712,6 +1762,9 @@
                 <c:pt idx="0">
                   <c:v>5112.0</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>10089.33333333333</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1777,6 +1830,9 @@
                 <c:pt idx="0">
                   <c:v>3692.5</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>7165.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1841,6 +1897,9 @@
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>4535.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9868.666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1969,7 +2028,7 @@
         <c:axId val="-2009028368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6000.0"/>
+          <c:max val="11000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4557,14 +4616,26 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_1" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_1" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr_1" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -4833,13 +4904,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -4890,26 +4962,39 @@
         <f>AVERAGE(B4:B11)</f>
         <v>5112</v>
       </c>
-      <c r="H2" s="6">
+      <c r="D2">
+        <f t="shared" ref="C2:F2" si="0">AVERAGE(D4:D11)</f>
+        <v>10089.333333333334</v>
+      </c>
+      <c r="H2" s="5">
         <f>AVERAGE(H4:H11)</f>
         <v>17.316149794937647</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="M2" s="9">
+      <c r="I2" s="5" t="e">
+        <f t="shared" ref="I2:K2" si="1">AVERAGE(I4:I11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J2" s="5">
+        <f>AVERAGE(J4:J11)</f>
+        <v>8.623344360590389</v>
+      </c>
+      <c r="K2" s="5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M2" s="8">
         <v>870</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="8">
         <v>870</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="8">
         <v>870</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="8">
         <v>870</v>
       </c>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -4919,21 +5004,33 @@
         <f>_xlfn.STDEV.S(B4:B11)</f>
         <v>723.10303553504741</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="H3" s="7">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <f t="shared" ref="C3:F3" si="2">_xlfn.STDEV.S(D4:D11)</f>
+        <v>81.794457839962078</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="H3" s="6">
         <f>_xlfn.STDEV.S(H4:H11)</f>
         <v>2.8067240187072193</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
+      <c r="I3" s="6" t="e">
+        <f t="shared" ref="I3:K3" si="3">_xlfn.STDEV.S(I4:I11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="6">
+        <f>_xlfn.STDEV.S(J4:J11)</f>
+        <v>6.9608164785766216E-2</v>
+      </c>
+      <c r="K3" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -4942,26 +5039,38 @@
       <c r="B4">
         <v>5525</v>
       </c>
-      <c r="H4" s="8">
+      <c r="D4">
+        <v>10032</v>
+      </c>
+      <c r="H4" s="7">
         <f>(M4/B4)*100</f>
         <v>15.746606334841628</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="M4" s="9">
+      <c r="I4" s="7" t="e">
+        <f t="shared" ref="I4:K6" si="4">(N4/C4)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="4"/>
+        <v>8.6722488038277508</v>
+      </c>
+      <c r="K4" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" s="8">
         <v>870</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="8">
         <v>870</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="8">
         <v>870</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>870</v>
       </c>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -4970,26 +5079,32 @@
       <c r="B5">
         <v>4052</v>
       </c>
-      <c r="H5" s="8">
-        <f t="shared" ref="H5:H11" si="0">(M5/B5)*100</f>
+      <c r="D5">
+        <v>10183</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" ref="H5:H11" si="5">(M5/B5)*100</f>
         <v>21.470878578479763</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="M5" s="9">
+      <c r="I5" s="7"/>
+      <c r="J5" s="7">
+        <f>(O5/D5)*100</f>
+        <v>8.5436511833447906</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="M5" s="8">
         <v>870</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>870</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <v>870</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>870</v>
       </c>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="8"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -4998,26 +5113,32 @@
       <c r="B6">
         <v>5255</v>
       </c>
-      <c r="H6" s="8">
-        <f t="shared" si="0"/>
+      <c r="D6">
+        <v>10053</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="5"/>
         <v>16.555661274976213</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="M6" s="9">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
+        <f>(O6/D6)*100</f>
+        <v>8.6541330945986275</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="M6" s="8">
         <v>870</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="8">
         <v>870</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="8">
         <v>870</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="8">
         <v>870</v>
       </c>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -5026,110 +5147,110 @@
       <c r="B7">
         <v>5616</v>
       </c>
-      <c r="H7" s="8">
-        <f t="shared" si="0"/>
+      <c r="H7" s="7">
+        <f t="shared" si="5"/>
         <v>15.491452991452991</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="M7" s="9">
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="M7" s="8">
         <v>870</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="8">
         <v>870</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="8">
         <v>870</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="8">
         <v>870</v>
       </c>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="M8" s="9">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="M8" s="8">
         <v>870</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="8">
         <v>870</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="8">
         <v>870</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="8">
         <v>870</v>
       </c>
-      <c r="Q8" s="9"/>
+      <c r="Q8" s="8"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="M9" s="9">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="M9" s="8">
         <v>870</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="8">
         <v>870</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="8">
         <v>870</v>
       </c>
-      <c r="P9" s="9">
+      <c r="P9" s="8">
         <v>870</v>
       </c>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="8"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="M10" s="9">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="M10" s="8">
         <v>870</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="8">
         <v>870</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="8">
         <v>870</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="8">
         <v>870</v>
       </c>
-      <c r="Q10" s="9"/>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="M11" s="9">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="M11" s="8">
         <v>870</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="8">
         <v>870</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="8">
         <v>870</v>
       </c>
-      <c r="P11" s="9">
+      <c r="P11" s="8">
         <v>870</v>
       </c>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5141,12 +5262,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -5172,6 +5294,10 @@
         <f>AVERAGE(B4:B11)</f>
         <v>3692.5</v>
       </c>
+      <c r="D2">
+        <f t="shared" ref="C2:E2" si="0">AVERAGE(D4:D11)</f>
+        <v>7165</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5181,9 +5307,12 @@
         <f>_xlfn.STDEV.S(B4:B11)</f>
         <v>890.74519364406342</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <f t="shared" ref="C3:E3" si="1">_xlfn.STDEV.S(D4:D11)</f>
+        <v>393.16027266243469</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -5192,6 +5321,9 @@
       <c r="B4">
         <v>2892</v>
       </c>
+      <c r="D4">
+        <v>7270</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -5200,6 +5332,9 @@
       <c r="B5">
         <v>3033</v>
       </c>
+      <c r="D5">
+        <v>7495</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -5207,6 +5342,9 @@
       </c>
       <c r="B6">
         <v>4077</v>
+      </c>
+      <c r="D6">
+        <v>6730</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -5247,12 +5385,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -5278,6 +5417,10 @@
         <f>AVERAGE(B4:B11)</f>
         <v>4535.25</v>
       </c>
+      <c r="D2">
+        <f t="shared" ref="C2:E2" si="0">AVERAGE(D4:D11)</f>
+        <v>9868.6666666666661</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5287,9 +5430,12 @@
         <f>_xlfn.STDEV.S(B4:B11)</f>
         <v>775.6100287300743</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <f t="shared" ref="C3:E3" si="1">_xlfn.STDEV.S(D4:D11)</f>
+        <v>89.628864398325007</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -5298,6 +5444,9 @@
       <c r="B4">
         <v>4953</v>
       </c>
+      <c r="D4">
+        <v>9812</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -5306,6 +5455,9 @@
       <c r="B5">
         <v>3393</v>
       </c>
+      <c r="D5">
+        <v>9972</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -5313,6 +5465,9 @@
       </c>
       <c r="B6">
         <v>4720</v>
+      </c>
+      <c r="D6">
+        <v>9822</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -5352,19 +5507,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:A35"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Iteration diagram integrated experiment
</commit_message>
<xml_diff>
--- a/viveks_workflow/analysis/integration_analysis.xlsx
+++ b/viveks_workflow/analysis/integration_analysis.xlsx
@@ -22,11 +22,11 @@
   </externalReferences>
   <definedNames>
     <definedName name="Te_Executing_task_aimes_emgr" localSheetId="2">Te!$B$4:$B$7</definedName>
-    <definedName name="Te_Executing_task_aimes_emgr_1" localSheetId="2">Te!$D$4:$D$6</definedName>
+    <definedName name="Te_Executing_task_aimes_emgr_1" localSheetId="2">Te!$D$4:$D$7</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr" localSheetId="0">TTC!$B$4:$B$7</definedName>
-    <definedName name="TTC_Time_to_completion_aimes_emgr_1" localSheetId="0">TTC!$D$4:$D$6</definedName>
+    <definedName name="TTC_Time_to_completion_aimes_emgr_1" localSheetId="0">TTC!$D$4:$D$7</definedName>
     <definedName name="Tw_Submitting_task_aimes_emgr" localSheetId="1">Tw!$B$4:$B$7</definedName>
-    <definedName name="Tw_Submitting_task_aimes_emgr_1" localSheetId="1">Tw!$D$4:$D$6</definedName>
+    <definedName name="Tw_Submitting_task_aimes_emgr_1" localSheetId="1">Tw!$D$4:$D$7</definedName>
   </definedNames>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -305,7 +305,7 @@
                     <c:v>723.1030355350474</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>81.79445783996207</c:v>
+                    <c:v>383.6903048032358</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -320,7 +320,7 @@
                     <c:v>723.1030355350474</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>81.79445783996207</c:v>
+                    <c:v>383.6903048032358</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -370,7 +370,7 @@
                   <c:v>5112.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10089.33333333333</c:v>
+                  <c:v>10278.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,7 +837,7 @@
                     <c:v>890.7451936440634</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>393.1602726624347</c:v>
+                    <c:v>321.463839335002</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -852,7 +852,7 @@
                     <c:v>890.7451936440634</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>393.1602726624347</c:v>
+                    <c:v>321.463839335002</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -902,7 +902,7 @@
                   <c:v>3692.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7165.0</c:v>
+                  <c:v>7156.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1292,7 +1292,7 @@
                     <c:v>775.6100287300743</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>89.62886439832501</c:v>
+                    <c:v>184.0115485506277</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1307,7 +1307,7 @@
                     <c:v>775.6100287300743</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>89.62886439832501</c:v>
+                    <c:v>184.0115485506277</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1357,7 +1357,7 @@
                   <c:v>4535.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9868.666666666666</c:v>
+                  <c:v>9784.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1732,6 +1732,55 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>TTC!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>723.1030355350474</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>383.6903048032358</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>TTC!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>723.1030355350474</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>383.6903048032358</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>TTC!$B$1:$E$1</c:f>
@@ -1763,7 +1812,7 @@
                   <c:v>5112.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10089.33333333333</c:v>
+                  <c:v>10278.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1777,7 +1826,7 @@
             <c:v>Tw</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1831,75 +1880,7 @@
                   <c:v>3692.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7165.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Te+Ts</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>TTC!$B$1:$E$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2048.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Te!$B$2:$E$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4535.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9868.666666666666</c:v>
+                  <c:v>7156.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2028,7 +2009,7 @@
         <c:axId val="-2009028368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="11000.0"/>
+          <c:max val="12000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4905,7 +4886,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4963,25 +4944,19 @@
         <v>5112</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="C2:F2" si="0">AVERAGE(D4:D11)</f>
-        <v>10089.333333333334</v>
+        <f>AVERAGE(D4:D12)</f>
+        <v>10278.25</v>
       </c>
       <c r="H2" s="5">
         <f>AVERAGE(H4:H11)</f>
         <v>17.316149794937647</v>
       </c>
-      <c r="I2" s="5" t="e">
-        <f t="shared" ref="I2:K2" si="1">AVERAGE(I4:I11)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="5">
         <f>AVERAGE(J4:J11)</f>
-        <v>8.623344360590389</v>
-      </c>
-      <c r="K2" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>8.412676667001266</v>
+      </c>
+      <c r="K2" s="5"/>
       <c r="M2" s="8">
         <v>870</v>
       </c>
@@ -5006,8 +4981,8 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
-        <f t="shared" ref="C3:F3" si="2">_xlfn.STDEV.S(D4:D11)</f>
-        <v>81.794457839962078</v>
+        <f>_xlfn.STDEV.S(D4:D12)</f>
+        <v>383.69030480323579</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -5015,18 +4990,12 @@
         <f>_xlfn.STDEV.S(H4:H11)</f>
         <v>2.8067240187072193</v>
       </c>
-      <c r="I3" s="6" t="e">
-        <f t="shared" ref="I3:K3" si="3">_xlfn.STDEV.S(I4:I11)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="I3" s="6"/>
       <c r="J3" s="6">
         <f>_xlfn.STDEV.S(J4:J11)</f>
-        <v>6.9608164785766216E-2</v>
-      </c>
-      <c r="K3" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>0.3442809219593656</v>
+      </c>
+      <c r="K3" s="6"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -5046,18 +5015,12 @@
         <f>(M4/B4)*100</f>
         <v>15.746606334841628</v>
       </c>
-      <c r="I4" s="7" t="e">
-        <f t="shared" ref="I4:K6" si="4">(N4/C4)*100</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="I4" s="7"/>
       <c r="J4" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I4:K4" si="0">(O4/D4)*100</f>
         <v>8.6722488038277508</v>
       </c>
-      <c r="K4" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K4" s="7"/>
       <c r="M4" s="8">
         <v>870</v>
       </c>
@@ -5083,7 +5046,7 @@
         <v>10183</v>
       </c>
       <c r="H5" s="7">
-        <f t="shared" ref="H5:H11" si="5">(M5/B5)*100</f>
+        <f t="shared" ref="H5:H7" si="1">(M5/B5)*100</f>
         <v>21.470878578479763</v>
       </c>
       <c r="I5" s="7"/>
@@ -5117,13 +5080,13 @@
         <v>10053</v>
       </c>
       <c r="H6" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>16.555661274976213</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7">
-        <f>(O6/D6)*100</f>
-        <v>8.6541330945986275</v>
+        <f>(O6/D7)*100</f>
+        <v>8.0221300138312586</v>
       </c>
       <c r="K6" s="7"/>
       <c r="M6" s="8">
@@ -5147,8 +5110,11 @@
       <c r="B7">
         <v>5616</v>
       </c>
+      <c r="D7">
+        <v>10845</v>
+      </c>
       <c r="H7" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>15.491452991452991</v>
       </c>
       <c r="I7" s="7"/>
@@ -5295,8 +5261,8 @@
         <v>3692.5</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="C2:E2" si="0">AVERAGE(D4:D11)</f>
-        <v>7165</v>
+        <f>AVERAGE(D4:D12)</f>
+        <v>7156.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5309,8 +5275,8 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
-        <f t="shared" ref="C3:E3" si="1">_xlfn.STDEV.S(D4:D11)</f>
-        <v>393.16027266243469</v>
+        <f>_xlfn.STDEV.S(D4:D12)</f>
+        <v>321.46383933500204</v>
       </c>
       <c r="E3" s="4"/>
     </row>
@@ -5353,6 +5319,9 @@
       </c>
       <c r="B7">
         <v>4768</v>
+      </c>
+      <c r="D7">
+        <v>7131</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5418,8 +5387,8 @@
         <v>4535.25</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="C2:E2" si="0">AVERAGE(D4:D11)</f>
-        <v>9868.6666666666661</v>
+        <f>AVERAGE(D4:D12)</f>
+        <v>9784.25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5432,8 +5401,8 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4">
-        <f t="shared" ref="C3:E3" si="1">_xlfn.STDEV.S(D4:D11)</f>
-        <v>89.628864398325007</v>
+        <f>_xlfn.STDEV.S(D4:D12)</f>
+        <v>184.01154855062765</v>
       </c>
       <c r="E3" s="4"/>
     </row>
@@ -5476,6 +5445,9 @@
       </c>
       <c r="B7">
         <v>5075</v>
+      </c>
+      <c r="D7">
+        <v>9531</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5507,7 +5479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:A35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Analysis and raw data 2048 simulations integration experiments
</commit_message>
<xml_diff>
--- a/viveks_workflow/analysis/integration_analysis.xlsx
+++ b/viveks_workflow/analysis/integration_analysis.xlsx
@@ -23,10 +23,13 @@
   <definedNames>
     <definedName name="Te_Executing_task_aimes_emgr" localSheetId="2">Te!$B$4:$B$7</definedName>
     <definedName name="Te_Executing_task_aimes_emgr_1" localSheetId="2">Te!$D$4:$D$7</definedName>
+    <definedName name="Te_Executing_task_aimes_emgr_2" localSheetId="2">Te!$E$4:$E$5</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr" localSheetId="0">TTC!$B$4:$B$7</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr_1" localSheetId="0">TTC!$D$4:$D$7</definedName>
+    <definedName name="TTC_Time_to_completion_aimes_emgr_2" localSheetId="0">TTC!$E$4:$E$5</definedName>
     <definedName name="Tw_Submitting_task_aimes_emgr" localSheetId="1">Tw!$B$4:$B$7</definedName>
     <definedName name="Tw_Submitting_task_aimes_emgr_1" localSheetId="1">Tw!$D$4:$D$7</definedName>
+    <definedName name="Tw_Submitting_task_aimes_emgr_2" localSheetId="1">Tw!$E$4:$E$5</definedName>
   </definedNames>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -42,8 +45,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Te-Executing_task-aimes_emgr" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/Te-Executing_task-aimes_emgr.csv">
+  <connection id="1" name="Te-Executing_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/Te-Executing_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
@@ -56,29 +59,50 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="TTC-Time_to_completion-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="3" name="Te-Executing_task-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/2048/Te-Executing_task-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="TTC-Time_to_completion-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="TTC-Time_to_completion-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="5" name="TTC-Time_to_completion-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="Tw-Submitting_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="6" name="TTC-Time_to_completion-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/2048/TTC-Time_to_completion-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="Tw-Submitting_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/Tw-Submitting_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="Tw-Submitting_task-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="8" name="Tw-Submitting_task-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/Tw-Submitting_task-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="Tw-Submitting_task-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/2048/Tw-Submitting_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
@@ -307,6 +331,9 @@
                   <c:pt idx="2">
                     <c:v>383.6903048032358</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -321,6 +348,9 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>383.6903048032358</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -371,6 +401,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10278.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23891.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -839,6 +872,9 @@
                   <c:pt idx="2">
                     <c:v>321.463839335002</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -853,6 +889,9 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>321.463839335002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -903,6 +942,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7156.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13819.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,6 +1336,9 @@
                   <c:pt idx="2">
                     <c:v>184.0115485506277</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -1308,6 +1353,9 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>184.0115485506277</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1358,6 +1406,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9784.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20659.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1749,6 +1800,9 @@
                   <c:pt idx="2">
                     <c:v>383.6903048032358</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -1763,6 +1817,9 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>383.6903048032358</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1813,6 +1870,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10278.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23891.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,6 +1941,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7156.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13819.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2009,7 +2072,7 @@
         <c:axId val="-2009028368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12000.0"/>
+          <c:max val="26000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4597,27 +4660,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_1" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_2" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_1" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_1" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_2" refreshOnLoad="1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_1" refreshOnLoad="1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr" refreshOnLoad="1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr_2" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr_1" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4886,13 +4961,13 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" customWidth="1"/>
+    <col min="4" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -4947,6 +5022,10 @@
         <f>AVERAGE(D4:D12)</f>
         <v>10278.25</v>
       </c>
+      <c r="E2">
+        <f>AVERAGE(E4:E12)</f>
+        <v>23891</v>
+      </c>
       <c r="H2" s="5">
         <f>AVERAGE(H4:H11)</f>
         <v>17.316149794937647</v>
@@ -4956,7 +5035,10 @@
         <f>AVERAGE(J4:J11)</f>
         <v>8.412676667001266</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="5">
+        <f>AVERAGE(K4:K11)</f>
+        <v>3.6415386547235364</v>
+      </c>
       <c r="M2" s="8">
         <v>870</v>
       </c>
@@ -4984,7 +5066,10 @@
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>383.69030480323579</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="e">
+        <f>_xlfn.STDEV.S(E4:E12)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="H3" s="6">
         <f>_xlfn.STDEV.S(H4:H11)</f>
@@ -4995,7 +5080,10 @@
         <f>_xlfn.STDEV.S(J4:J11)</f>
         <v>0.3442809219593656</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6" t="e">
+        <f>_xlfn.STDEV.S(K4:K11)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -5011,6 +5099,9 @@
       <c r="D4">
         <v>10032</v>
       </c>
+      <c r="E4">
+        <v>23891</v>
+      </c>
       <c r="H4" s="7">
         <f>(M4/B4)*100</f>
         <v>15.746606334841628</v>
@@ -5020,7 +5111,10 @@
         <f t="shared" ref="I4:K4" si="0">(O4/D4)*100</f>
         <v>8.6722488038277508</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7">
+        <f t="shared" si="0"/>
+        <v>3.6415386547235364</v>
+      </c>
       <c r="M4" s="8">
         <v>870</v>
       </c>
@@ -5228,13 +5322,14 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -5264,6 +5359,10 @@
         <f>AVERAGE(D4:D12)</f>
         <v>7156.5</v>
       </c>
+      <c r="E2">
+        <f>AVERAGE(E4:E12)</f>
+        <v>13819</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5278,7 +5377,10 @@
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>321.46383933500204</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="e">
+        <f>_xlfn.STDEV.S(E4:E12)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -5289,6 +5391,9 @@
       </c>
       <c r="D4">
         <v>7270</v>
+      </c>
+      <c r="E4">
+        <v>13819</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -5354,13 +5459,14 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -5390,6 +5496,10 @@
         <f>AVERAGE(D4:D12)</f>
         <v>9784.25</v>
       </c>
+      <c r="E2">
+        <f>AVERAGE(E4:E12)</f>
+        <v>20659</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5404,7 +5514,10 @@
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>184.01154855062765</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="e">
+        <f>_xlfn.STDEV.S(E4:E12)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -5415,6 +5528,9 @@
       </c>
       <c r="D4">
         <v>9812</v>
+      </c>
+      <c r="E4">
+        <v>20659</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Complete analysis 2048 simulations integrated experiments. Analysis 512 first run
</commit_message>
<xml_diff>
--- a/viveks_workflow/analysis/integration_analysis.xlsx
+++ b/viveks_workflow/analysis/integration_analysis.xlsx
@@ -23,16 +23,19 @@
   <definedNames>
     <definedName name="Te_Executing_task_aimes_emgr" localSheetId="2">Te!$B$4:$B$7</definedName>
     <definedName name="Te_Executing_task_aimes_emgr_1" localSheetId="2">Te!$D$4:$D$7</definedName>
-    <definedName name="Te_Executing_task_aimes_emgr_2" localSheetId="2">Te!$E$4:$E$5</definedName>
+    <definedName name="Te_Executing_task_aimes_emgr_2" localSheetId="2">Te!$E$4:$E$7</definedName>
+    <definedName name="Te_Executing_task_aimes_emgr_3" localSheetId="2">Te!$C$4:$C$5</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr" localSheetId="0">TTC!$B$4:$B$7</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr_1" localSheetId="0">TTC!$D$4:$D$7</definedName>
-    <definedName name="TTC_Time_to_completion_aimes_emgr_2" localSheetId="0">TTC!$E$4:$E$5</definedName>
-    <definedName name="TTC_Time_to_completion_aimes_emgr_3" localSheetId="0">TTC!$U$4:$U$5</definedName>
+    <definedName name="TTC_Time_to_completion_aimes_emgr_2" localSheetId="0">TTC!$E$4:$E$7</definedName>
+    <definedName name="TTC_Time_to_completion_aimes_emgr_3" localSheetId="0">TTC!$U$4:$U$7</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr_4" localSheetId="0">TTC!$T$4:$T$7</definedName>
     <definedName name="TTC_Time_to_completion_aimes_emgr_5" localSheetId="0">TTC!$S$4:$S$7</definedName>
+    <definedName name="TTC_Time_to_completion_aimes_emgr_6" localSheetId="0">TTC!$C$4:$C$5</definedName>
     <definedName name="Tw_Submitting_task_aimes_emgr" localSheetId="1">Tw!$B$4:$B$7</definedName>
     <definedName name="Tw_Submitting_task_aimes_emgr_1" localSheetId="1">Tw!$D$4:$D$7</definedName>
-    <definedName name="Tw_Submitting_task_aimes_emgr_2" localSheetId="1">Tw!$E$4:$E$5</definedName>
+    <definedName name="Tw_Submitting_task_aimes_emgr_2" localSheetId="1">Tw!$E$4:$E$7</definedName>
+    <definedName name="Tw_Submitting_task_aimes_emgr_3" localSheetId="1">Tw!$C$4:$C$5</definedName>
   </definedNames>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -69,64 +72,85 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="TTC-Time_to_completion-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="4" name="Te-Executing_task-aimes_emgr3" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/512/Te-Executing_task-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="TTC-Time_to_completion-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="TTC-Time_to_completion-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="6" name="TTC-Time_to_completion-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="TTC-Time_to_completion-aimes_emgr11" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="7" name="TTC-Time_to_completion-aimes_emgr11" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="TTC-Time_to_completion-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="8" name="TTC-Time_to_completion-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/2048/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="TTC-Time_to_completion-aimes_emgr21" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="9" name="TTC-Time_to_completion-aimes_emgr21" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/2048/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="TTC-Time_to_completion-aimes_emgr3" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="10" name="TTC-Time_to_completion-aimes_emgr3" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/TTC-Time_to_completion-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="Tw-Submitting_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="11" name="TTC-Time_to_completion-aimes_emgr4" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/512/TTC-Time_to_completion-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="12" name="Tw-Submitting_task-aimes_emgr" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/256/Tw-Submitting_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="Tw-Submitting_task-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="13" name="Tw-Submitting_task-aimes_emgr1" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/1024/Tw-Submitting_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="Tw-Submitting_task-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="14" name="Tw-Submitting_task-aimes_emgr2" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/2048/Tw-Submitting_task-aimes_emgr.csv">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="15" name="Tw-Submitting_task-aimes_emgr3" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/aimes.swift.experiments/viveks_workflow/analysis/512/Tw-Submitting_task-aimes_emgr.csv">
       <textFields>
         <textField/>
       </textFields>
@@ -372,11 +396,14 @@
                   <c:pt idx="0">
                     <c:v>723.1030355350474</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>557.3490827120827</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>938.3306986345485</c:v>
+                    <c:v>696.3568888627918</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -390,11 +417,14 @@
                   <c:pt idx="0">
                     <c:v>723.1030355350474</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>557.3490827120827</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>938.3306986345485</c:v>
+                    <c:v>696.3568888627918</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -443,11 +473,14 @@
                 <c:pt idx="0">
                   <c:v>5112.0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>7091.0</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>10366.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23227.5</c:v>
+                  <c:v>23563.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,11 +946,14 @@
                   <c:pt idx="0">
                     <c:v>890.7451936440634</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>321.463839335002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.121320343559642</c:v>
+                    <c:v>463.6399465102203</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -931,11 +967,14 @@
                   <c:pt idx="0">
                     <c:v>890.7451936440634</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>321.463839335002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.121320343559642</c:v>
+                    <c:v>463.6399465102203</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -984,11 +1023,14 @@
                 <c:pt idx="0">
                   <c:v>3692.5</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>5179.0</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>7156.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13817.5</c:v>
+                  <c:v>14111.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1377,11 +1419,14 @@
                   <c:pt idx="0">
                     <c:v>775.6100287300743</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>184.0115485506277</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>956.0083681642122</c:v>
+                    <c:v>649.2115731151646</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1395,11 +1440,14 @@
                   <c:pt idx="0">
                     <c:v>775.6100287300743</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
                   <c:pt idx="2">
                     <c:v>184.0115485506277</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>956.0083681642122</c:v>
+                    <c:v>649.2115731151646</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1448,11 +1496,14 @@
                 <c:pt idx="0">
                   <c:v>4535.25</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>6146.0</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>9784.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19983.0</c:v>
+                  <c:v>20265.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,7 +1896,7 @@
                     <c:v>557.3490827120827</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>938.3306986345485</c:v>
+                    <c:v>696.3568888627918</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1863,7 +1914,7 @@
                     <c:v>557.3490827120827</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>938.3306986345485</c:v>
+                    <c:v>696.3568888627918</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1884,17 +1935,20 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(TTC!$B$1,TTC!$D$1,TTC!$E$1)</c:f>
+              <c:f>TTC!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1024.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1902,18 +1956,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(TTC!$B$2,TTC!$D$2,TTC!$E$2)</c:f>
+              <c:f>TTC!$B$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5112.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7091.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10366.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>23227.5</c:v>
+                <c:pt idx="3">
+                  <c:v>23563.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1921,21 +1978,13 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>plots!$W$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>TTCi</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1960,17 +2009,20 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(TTC!$B$1,TTC!$D$1,TTC!$E$1)</c:f>
+              <c:f>TTC!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1024.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2048.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1978,18 +2030,150 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tw!$B$2,Tw!$D$2,Tw!$E$2)</c:f>
+              <c:f>TTC!$M$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>870.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>870.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>870.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>870.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Tw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Tw!$B$3,Tw!$D$3,Tw!$E$3)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>890.7451936440634</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>321.463839335002</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>463.6399465102203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Tw!$B$3,Tw!$D$3,Tw!$E$3)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>890.7451936440634</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>321.463839335002</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>463.6399465102203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTC!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tw!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3692.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5179.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>7156.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>13817.5</c:v>
+                <c:pt idx="3">
+                  <c:v>14111.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2271,7 +2455,7 @@
           <a:pPr>
             <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:latin typeface="NimbusRomNo9L" charset="0"/>
               <a:ea typeface="NimbusRomNo9L" charset="0"/>
@@ -2311,6 +2495,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4619,6 +4804,95 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.90741</cdr:x>
+      <cdr:y>0.31794</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.99846</cdr:x>
+      <cdr:y>0.68709</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7467600" y="938396"/>
+          <a:ext cx="749300" cy="1089529"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="120000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="1">
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:rPr>
+            <a:t>TTC</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="120000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="1">
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:rPr>
+            <a:t>TTCi</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="120000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="1">
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:rPr>
+            <a:t>T</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="1" baseline="-25000">
+              <a:latin typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:ea typeface="Nimbus Roman Becker No9L" charset="0"/>
+              <a:cs typeface="Nimbus Roman Becker No9L" charset="0"/>
+            </a:rPr>
+            <a:t>w</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -4706,51 +4980,63 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_5" refreshOnLoad="1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_6" refreshOnLoad="1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_1" refreshOnLoad="1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr" refreshOnLoad="1" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr_3" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr_2" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr_1" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-aimes_emgr" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_4" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_5" refreshOnLoad="1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_3" refreshOnLoad="1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_4" refreshOnLoad="1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_2" refreshOnLoad="1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_3" refreshOnLoad="1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_1" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_2" refreshOnLoad="1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr_1" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_2" refreshOnLoad="1" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-aimes_emgr" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_1" refreshOnLoad="1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_3" refreshOnLoad="1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr" refreshOnLoad="1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-aimes_emgr_2" refreshOnLoad="1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5018,14 +5304,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="2" max="3" width="5.1640625" customWidth="1"/>
     <col min="4" max="5" width="6.1640625" customWidth="1"/>
+    <col min="19" max="19" width="5.1640625" customWidth="1"/>
+    <col min="20" max="21" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -5086,26 +5374,33 @@
         <f>AVERAGE(B4:B11)</f>
         <v>5112</v>
       </c>
+      <c r="C2">
+        <f>AVERAGE(C4:C11)</f>
+        <v>7091</v>
+      </c>
       <c r="D2">
         <f>AVERAGE(D4:D12)</f>
         <v>10366</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E4:E12)</f>
-        <v>23227.5</v>
+        <f>AVERAGE(E4:E14)</f>
+        <v>23563.75</v>
       </c>
       <c r="H2" s="5">
         <f>AVERAGE(H4:H11)</f>
         <v>17.316149794937647</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="5">
+        <f>AVERAGE(I4:I11)</f>
+        <v>12.269073473417007</v>
+      </c>
       <c r="J2" s="5">
         <f>AVERAGE(J4:J11)</f>
-        <v>8.3288441186252165</v>
+        <v>8.4101663626185683</v>
       </c>
       <c r="K2" s="5">
         <f>AVERAGE(K4:K11)</f>
-        <v>3.748618999405732</v>
+        <v>3.6945875994325386</v>
       </c>
       <c r="M2" s="8">
         <v>870</v>
@@ -5132,8 +5427,8 @@
         <v>10366</v>
       </c>
       <c r="U2">
-        <f>AVERAGE(U4:U12)</f>
-        <v>23227.5</v>
+        <f>AVERAGE(U4:U14)</f>
+        <v>23563.75</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -5144,28 +5439,34 @@
         <f>_xlfn.STDEV.S(B4:B11)</f>
         <v>723.10303553504741</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="e">
+        <f>_xlfn.STDEV.S(C4:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="D3" s="4">
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>557.34908271208269</v>
       </c>
       <c r="E3" s="4">
-        <f>_xlfn.STDEV.S(E4:E12)</f>
-        <v>938.33069863454853</v>
+        <f>_xlfn.STDEV.S(E4:E14)</f>
+        <v>696.35688886279183</v>
       </c>
       <c r="F3" s="4"/>
       <c r="H3" s="6">
         <f>_xlfn.STDEV.S(H4:H11)</f>
         <v>2.8067240187072193</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="6" t="e">
+        <f>_xlfn.STDEV.S(I4:I11)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="J3" s="6">
         <f>_xlfn.STDEV.S(J4:J11)</f>
-        <v>0.48768289421692529</v>
+        <v>0.43012746135727647</v>
       </c>
       <c r="K3" s="6">
         <f>_xlfn.STDEV.S(K4:K11)</f>
-        <v>0.15143447571314664</v>
+        <v>0.11171559683572883</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -5183,8 +5484,8 @@
         <v>557.34908271208269</v>
       </c>
       <c r="U3" s="4">
-        <f>_xlfn.STDEV.S(U4:U12)</f>
-        <v>938.33069863454853</v>
+        <f>_xlfn.STDEV.S(U4:U14)</f>
+        <v>696.35688886279183</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -5194,6 +5495,9 @@
       <c r="B4">
         <v>5525</v>
       </c>
+      <c r="C4">
+        <v>7091</v>
+      </c>
       <c r="D4">
         <v>10032</v>
       </c>
@@ -5204,9 +5508,12 @@
         <f>(M4/B4)*100</f>
         <v>15.746606334841628</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7">
+        <f>(N4/C4)*100</f>
+        <v>12.269073473417007</v>
+      </c>
       <c r="J4" s="7">
-        <f t="shared" ref="I4:K5" si="0">(O4/D4)*100</f>
+        <f t="shared" ref="J4:K7" si="0">(O4/D4)*100</f>
         <v>8.6722488038277508</v>
       </c>
       <c r="K4" s="7">
@@ -5258,7 +5565,7 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7">
-        <f>(O5/D5)*100</f>
+        <f t="shared" si="0"/>
         <v>8.5436511833447906</v>
       </c>
       <c r="K5" s="7">
@@ -5301,16 +5608,22 @@
       <c r="D6">
         <v>10053</v>
       </c>
+      <c r="E6">
+        <v>23653</v>
+      </c>
       <c r="H6" s="7">
         <f t="shared" si="1"/>
         <v>16.555661274976213</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7">
-        <f>(O6/D7)*100</f>
-        <v>7.770632368703108</v>
-      </c>
-      <c r="K6" s="7"/>
+        <f t="shared" si="0"/>
+        <v>8.6541330945986275</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="0"/>
+        <v>3.678180357671331</v>
+      </c>
       <c r="M6" s="8">
         <v>870</v>
       </c>
@@ -5332,6 +5645,9 @@
       </c>
       <c r="T6">
         <v>10053</v>
+      </c>
+      <c r="U6">
+        <v>23653</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -5344,13 +5660,22 @@
       <c r="D7">
         <v>11196</v>
       </c>
+      <c r="E7">
+        <v>24147</v>
+      </c>
       <c r="H7" s="7">
         <f t="shared" si="1"/>
         <v>15.491452991452991</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="J7" s="7">
+        <f>(O7/D7)*100</f>
+        <v>7.770632368703108</v>
+      </c>
+      <c r="K7" s="7">
+        <f>(P7/E7)*100</f>
+        <v>3.6029320412473602</v>
+      </c>
       <c r="M7" s="8">
         <v>870</v>
       </c>
@@ -5372,6 +5697,9 @@
       </c>
       <c r="T7">
         <v>11196</v>
+      </c>
+      <c r="U7">
+        <v>24147</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -5480,13 +5808,12 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="2" max="4" width="5.1640625" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5513,13 +5840,17 @@
         <f>AVERAGE(B4:B11)</f>
         <v>3692.5</v>
       </c>
+      <c r="C2">
+        <f>AVERAGE(C4:C11)</f>
+        <v>5179</v>
+      </c>
       <c r="D2">
         <f>AVERAGE(D4:D12)</f>
         <v>7156.5</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E4:E12)</f>
-        <v>13817.5</v>
+        <f>AVERAGE(E4:E14)</f>
+        <v>14111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5530,14 +5861,17 @@
         <f>_xlfn.STDEV.S(B4:B11)</f>
         <v>890.74519364406342</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="e">
+        <f>_xlfn.STDEV.S(C4:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="D3" s="4">
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>321.46383933500204</v>
       </c>
       <c r="E3" s="4">
-        <f>_xlfn.STDEV.S(E4:E12)</f>
-        <v>2.1213203435596424</v>
+        <f>_xlfn.STDEV.S(E4:E14)</f>
+        <v>463.63994651022034</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -5547,6 +5881,9 @@
       <c r="B4">
         <v>2892</v>
       </c>
+      <c r="C4">
+        <v>5179</v>
+      </c>
       <c r="D4">
         <v>7270</v>
       </c>
@@ -5578,6 +5915,9 @@
       <c r="D6">
         <v>6730</v>
       </c>
+      <c r="E6">
+        <v>14017</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -5588,6 +5928,9 @@
       </c>
       <c r="D7">
         <v>7131</v>
+      </c>
+      <c r="E7">
+        <v>14792</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5620,13 +5963,12 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="2" max="4" width="5.1640625" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5653,13 +5995,17 @@
         <f>AVERAGE(B4:B11)</f>
         <v>4535.25</v>
       </c>
+      <c r="C2">
+        <f>AVERAGE(C4:C11)</f>
+        <v>6146</v>
+      </c>
       <c r="D2">
         <f>AVERAGE(D4:D12)</f>
         <v>9784.25</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E4:E12)</f>
-        <v>19983</v>
+        <f>AVERAGE(E4:E14)</f>
+        <v>20265.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5670,14 +6016,17 @@
         <f>_xlfn.STDEV.S(B4:B11)</f>
         <v>775.6100287300743</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="e">
+        <f>_xlfn.STDEV.S(C4:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="D3" s="4">
         <f>_xlfn.STDEV.S(D4:D12)</f>
         <v>184.01154855062765</v>
       </c>
       <c r="E3" s="4">
-        <f>_xlfn.STDEV.S(E4:E12)</f>
-        <v>956.00836816421224</v>
+        <f>_xlfn.STDEV.S(E4:E14)</f>
+        <v>649.21157311516458</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -5687,6 +6036,9 @@
       <c r="B4">
         <v>4953</v>
       </c>
+      <c r="C4">
+        <v>6146</v>
+      </c>
       <c r="D4">
         <v>9812</v>
       </c>
@@ -5718,6 +6070,9 @@
       <c r="D6">
         <v>9822</v>
       </c>
+      <c r="E6">
+        <v>20423</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -5728,6 +6083,9 @@
       </c>
       <c r="D7">
         <v>9531</v>
+      </c>
+      <c r="E7">
+        <v>20673</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5759,8 +6117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>